<commit_message>
Add line sensor ID
</commit_message>
<xml_diff>
--- a/R2CANIDList.xlsx
+++ b/R2CANIDList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tsemi\2023\ABURobocon2024\Software\NHK2024_R2CANIDList\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shibatakeigo/Development/t-semi/NHK2024_R2CANIDList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E996A3-B2E4-4A10-9B3C-5DD8B18B652F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011174A6-3F5F-234A-9465-13E55422E741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-6345" windowWidth="16440" windowHeight="29040" xr2:uid="{BB5A1F1B-FA35-4493-89FB-4447E27D9365}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BB5A1F1B-FA35-4493-89FB-4447E27D9365}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="46">
   <si>
     <t>hex</t>
     <phoneticPr fontId="1"/>
@@ -304,12 +304,39 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>(float)ラインからの横ずれ</t>
+    <rPh sb="13" eb="14">
+      <t>ヨコ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>(float)ロボットとラインのずれている角度</t>
+    <rPh sb="21" eb="23">
+      <t>カクド</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0: 通常 1: 水平ラインを検出</t>
+    <rPh sb="3" eb="5">
+      <t>ツウジョウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>スイヘイライ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ケンシュテゥ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,8 +409,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0B2A4BCC-9593-4525-8C08-B113DFFDAC55}" name="テーブル2" displayName="テーブル2" ref="A1:K44" totalsRowShown="0">
-  <autoFilter ref="A1:K44" xr:uid="{0B2A4BCC-9593-4525-8C08-B113DFFDAC55}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0B2A4BCC-9593-4525-8C08-B113DFFDAC55}" name="テーブル2" displayName="テーブル2" ref="A1:K46" totalsRowShown="0">
+  <autoFilter ref="A1:K46" xr:uid="{0B2A4BCC-9593-4525-8C08-B113DFFDAC55}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{DF83237B-E6E4-4C7E-A335-421521EC2352}" name="列1"/>
     <tableColumn id="2" xr3:uid="{8113689F-2AE8-4ABD-B1CB-D4DD87CB8EAF}" name="用途"/>
@@ -702,23 +729,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656D051C-6FCF-4257-9D0F-A5444B2232EC}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
   <cols>
-    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.375" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -753,7 +780,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -784,7 +811,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11">
       <c r="B3" t="s">
         <v>35</v>
       </c>
@@ -812,7 +839,7 @@
         <v>00000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -843,7 +870,7 @@
         <v>00000010</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -872,7 +899,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -900,7 +927,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11">
       <c r="I7" s="2"/>
       <c r="J7" t="str">
         <f t="shared" si="2"/>
@@ -911,7 +938,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11">
       <c r="I8" s="2"/>
       <c r="J8" t="str">
         <f t="shared" si="2"/>
@@ -922,7 +949,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11">
       <c r="I9" s="2"/>
       <c r="J9" t="str">
         <f t="shared" si="2"/>
@@ -933,7 +960,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11">
       <c r="I10" s="2"/>
       <c r="J10" t="str">
         <f t="shared" si="2"/>
@@ -944,7 +971,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -975,7 +1002,7 @@
         <v>00000010</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -1001,7 +1028,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -1027,7 +1054,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11">
       <c r="B14" t="s">
         <v>26</v>
       </c>
@@ -1053,7 +1080,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -1082,7 +1109,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -1108,7 +1135,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:11">
       <c r="I17" s="2"/>
       <c r="J17" t="str">
         <f t="shared" si="4"/>
@@ -1119,7 +1146,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:11">
       <c r="I18" s="2"/>
       <c r="J18" t="str">
         <f t="shared" si="4"/>
@@ -1130,7 +1157,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:11">
       <c r="I19" s="2"/>
       <c r="J19" t="str">
         <f t="shared" si="4"/>
@@ -1141,7 +1168,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:11">
       <c r="I20" s="2"/>
       <c r="J20" t="str">
         <f t="shared" si="4"/>
@@ -1152,7 +1179,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:11">
       <c r="I21" s="2"/>
       <c r="J21" t="str">
         <f t="shared" ref="J21:J23" si="6">HEX2BIN(H21,3)</f>
@@ -1163,7 +1190,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:11">
       <c r="I22" s="2"/>
       <c r="J22" t="str">
         <f t="shared" si="6"/>
@@ -1174,7 +1201,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:11">
       <c r="I23" s="2"/>
       <c r="J23" t="str">
         <f t="shared" si="6"/>
@@ -1185,7 +1212,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:11">
       <c r="I24" s="2"/>
       <c r="J24" t="str">
         <f t="shared" ref="J24" si="8">HEX2BIN(H24,3)</f>
@@ -1196,7 +1223,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:11">
       <c r="B25" t="s">
         <v>16</v>
       </c>
@@ -1206,95 +1233,130 @@
       <c r="E25">
         <v>1000</v>
       </c>
+      <c r="G25" t="s">
+        <v>43</v>
+      </c>
       <c r="H25">
         <v>2</v>
       </c>
-      <c r="I25" s="2"/>
+      <c r="I25" s="2">
+        <v>6</v>
+      </c>
       <c r="J25" t="str">
         <f>HEX2BIN(H25,3)</f>
         <v>010</v>
       </c>
       <c r="K25" t="str">
         <f>HEX2BIN(I25,8)</f>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.4">
+        <v>00000110</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11">
       <c r="B26" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="E26">
         <v>1000</v>
       </c>
-      <c r="H26">
-        <v>2</v>
-      </c>
-      <c r="I26" s="2"/>
+      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="2">
+        <v>7</v>
+      </c>
       <c r="J26" t="str">
         <f>HEX2BIN(H26,3)</f>
-        <v>010</v>
+        <v>000</v>
       </c>
       <c r="K26" t="str">
         <f>HEX2BIN(I26,8)</f>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="I27" s="2"/>
+        <v>00000111</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27">
+        <v>1000</v>
+      </c>
+      <c r="G27" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="2">
+        <v>8</v>
+      </c>
       <c r="J27" t="str">
         <f>HEX2BIN(H27,3)</f>
         <v>000</v>
       </c>
       <c r="K27" t="str">
         <f>HEX2BIN(I27,8)</f>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.4">
+        <v>00001000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28">
+        <v>1000</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
       <c r="I28" s="2"/>
       <c r="J28" t="str">
         <f>HEX2BIN(H28,3)</f>
-        <v>000</v>
+        <v>010</v>
       </c>
       <c r="K28" t="str">
         <f>HEX2BIN(I28,8)</f>
         <v>00000000</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:11">
+      <c r="I29" s="2"/>
       <c r="J29" t="str">
-        <f t="shared" ref="J29:J44" si="10">HEX2BIN(H29,3)</f>
+        <f>HEX2BIN(H29,3)</f>
         <v>000</v>
       </c>
       <c r="K29" t="str">
-        <f t="shared" ref="K29:K44" si="11">HEX2BIN(I29,8)</f>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.4">
+        <f>HEX2BIN(I29,8)</f>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="I30" s="2"/>
       <c r="J30" t="str">
-        <f t="shared" si="10"/>
+        <f>HEX2BIN(H30,3)</f>
         <v>000</v>
       </c>
       <c r="K30" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.4">
+        <f>HEX2BIN(I30,8)</f>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11">
       <c r="J31" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="J31:J46" si="10">HEX2BIN(H31,3)</f>
         <v>000</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.4">
+        <f t="shared" ref="K31:K46" si="11">HEX2BIN(I31,8)</f>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11">
       <c r="J32" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
@@ -1304,7 +1366,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="33" spans="2:11">
       <c r="J33" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
@@ -1314,7 +1376,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:11">
       <c r="J34" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
@@ -1324,7 +1386,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="2:11">
       <c r="J35" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
@@ -1334,35 +1396,17 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B36" t="s">
-        <v>23</v>
-      </c>
-      <c r="C36" t="s">
-        <v>36</v>
-      </c>
-      <c r="E36">
-        <v>1000</v>
-      </c>
-      <c r="F36">
-        <v>64</v>
-      </c>
-      <c r="H36">
-        <v>7</v>
-      </c>
-      <c r="I36">
-        <v>2</v>
-      </c>
+    <row r="36" spans="2:11">
       <c r="J36" t="str">
         <f t="shared" si="10"/>
-        <v>111</v>
+        <v>000</v>
       </c>
       <c r="K36" t="str">
         <f t="shared" si="11"/>
-        <v>00000010</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.4">
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11">
       <c r="J37" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
@@ -1372,17 +1416,35 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="2:11">
+      <c r="B38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38">
+        <v>1000</v>
+      </c>
+      <c r="F38">
+        <v>64</v>
+      </c>
+      <c r="H38">
+        <v>7</v>
+      </c>
+      <c r="I38">
+        <v>2</v>
+      </c>
       <c r="J38" t="str">
         <f t="shared" si="10"/>
-        <v>000</v>
+        <v>111</v>
       </c>
       <c r="K38" t="str">
         <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.4">
+        <v>00000010</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11">
       <c r="J39" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
@@ -1392,7 +1454,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:11">
       <c r="J40" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
@@ -1402,7 +1464,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="2:11">
       <c r="J41" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
@@ -1412,7 +1474,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="42" spans="2:11">
       <c r="J42" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
@@ -1422,7 +1484,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="2:11">
       <c r="J43" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
@@ -1432,12 +1494,32 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.4">
+    <row r="44" spans="2:11">
       <c r="J44" t="str">
         <f t="shared" si="10"/>
         <v>000</v>
       </c>
       <c r="K44" t="str">
+        <f t="shared" si="11"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="J45" t="str">
+        <f t="shared" si="10"/>
+        <v>000</v>
+      </c>
+      <c r="K45" t="str">
+        <f t="shared" si="11"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="J46" t="str">
+        <f t="shared" si="10"/>
+        <v>000</v>
+      </c>
+      <c r="K46" t="str">
         <f t="shared" si="11"/>
         <v>00000000</v>
       </c>
@@ -1682,18 +1764,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1716,14 +1798,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4BDA834-5B92-48FB-A6B0-E102C84F4220}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D12E982E-9C6D-41F1-B30C-74FFA2E58A60}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="10495901-9a88-43e9-a0c2-59df6c25c8bf"/>
@@ -1738,4 +1812,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4BDA834-5B92-48FB-A6B0-E102C84F4220}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add id for robot velocity
</commit_message>
<xml_diff>
--- a/R2CANIDList.xlsx
+++ b/R2CANIDList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shibatakeigo/Development/t-semi/NHK2024_R2CANIDList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tsemi\2023\ABURobocon2024\Software\NHK2024_R2CANIDList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{011174A6-3F5F-234A-9465-13E55422E741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05633631-D9C7-4B7A-AE73-112F6AC9B3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{BB5A1F1B-FA35-4493-89FB-4447E27D9365}"/>
+    <workbookView xWindow="-16320" yWindow="-6345" windowWidth="16440" windowHeight="29040" xr2:uid="{BB5A1F1B-FA35-4493-89FB-4447E27D9365}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -336,7 +336,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -433,9 +433,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -473,7 +473,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -579,7 +579,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -721,7 +721,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -731,21 +731,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{656D051C-6FCF-4257-9D0F-A5444B2232EC}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.375" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>29</v>
       </c>
@@ -780,7 +780,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B2" t="s">
         <v>9</v>
       </c>
@@ -811,7 +811,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B3" t="s">
         <v>35</v>
       </c>
@@ -839,7 +839,7 @@
         <v>00000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -870,7 +870,7 @@
         <v>00000010</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -899,7 +899,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B6" t="s">
         <v>21</v>
       </c>
@@ -927,7 +927,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="I7" s="2"/>
       <c r="J7" t="str">
         <f t="shared" si="2"/>
@@ -938,7 +938,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="I8" s="2"/>
       <c r="J8" t="str">
         <f t="shared" si="2"/>
@@ -949,7 +949,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="I9" s="2"/>
       <c r="J9" t="str">
         <f t="shared" si="2"/>
@@ -960,7 +960,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="I10" s="2"/>
       <c r="J10" t="str">
         <f t="shared" si="2"/>
@@ -971,7 +971,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B11" t="s">
         <v>12</v>
       </c>
@@ -991,7 +991,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J11" t="str">
         <f>HEX2BIN(H11,3)</f>
@@ -999,10 +999,10 @@
       </c>
       <c r="K11" t="str">
         <f>HEX2BIN(I11,8)</f>
-        <v>00000010</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>00000110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B12" t="s">
         <v>3</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B13" t="s">
         <v>4</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B14" t="s">
         <v>26</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="17" spans="2:11">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.4">
       <c r="I17" s="2"/>
       <c r="J17" t="str">
         <f t="shared" si="4"/>
@@ -1146,7 +1146,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="18" spans="2:11">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.4">
       <c r="I18" s="2"/>
       <c r="J18" t="str">
         <f t="shared" si="4"/>
@@ -1157,7 +1157,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="19" spans="2:11">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.4">
       <c r="I19" s="2"/>
       <c r="J19" t="str">
         <f t="shared" si="4"/>
@@ -1168,7 +1168,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="20" spans="2:11">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.4">
       <c r="I20" s="2"/>
       <c r="J20" t="str">
         <f t="shared" si="4"/>
@@ -1179,7 +1179,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="21" spans="2:11">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.4">
       <c r="I21" s="2"/>
       <c r="J21" t="str">
         <f t="shared" ref="J21:J23" si="6">HEX2BIN(H21,3)</f>
@@ -1190,7 +1190,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="22" spans="2:11">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.4">
       <c r="I22" s="2"/>
       <c r="J22" t="str">
         <f t="shared" si="6"/>
@@ -1201,7 +1201,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="23" spans="2:11">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.4">
       <c r="I23" s="2"/>
       <c r="J23" t="str">
         <f t="shared" si="6"/>
@@ -1212,7 +1212,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="24" spans="2:11">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.4">
       <c r="I24" s="2"/>
       <c r="J24" t="str">
         <f t="shared" ref="J24" si="8">HEX2BIN(H24,3)</f>
@@ -1223,7 +1223,7 @@
         <v>00000000</v>
       </c>
     </row>
-    <row r="25" spans="2:11">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B25" t="s">
         <v>16</v>
       </c>
@@ -1243,15 +1243,15 @@
         <v>6</v>
       </c>
       <c r="J25" t="str">
-        <f>HEX2BIN(H25,3)</f>
+        <f t="shared" ref="J25:J30" si="10">HEX2BIN(H25,3)</f>
         <v>010</v>
       </c>
       <c r="K25" t="str">
-        <f>HEX2BIN(I25,8)</f>
+        <f t="shared" ref="K25:K30" si="11">HEX2BIN(I25,8)</f>
         <v>00000110</v>
       </c>
     </row>
-    <row r="26" spans="2:11">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B26" t="s">
         <v>16</v>
       </c>
@@ -1268,15 +1268,15 @@
         <v>7</v>
       </c>
       <c r="J26" t="str">
-        <f>HEX2BIN(H26,3)</f>
+        <f t="shared" si="10"/>
         <v>000</v>
       </c>
       <c r="K26" t="str">
-        <f>HEX2BIN(I26,8)</f>
+        <f t="shared" si="11"/>
         <v>00000111</v>
       </c>
     </row>
-    <row r="27" spans="2:11">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>16</v>
       </c>
@@ -1293,15 +1293,15 @@
         <v>8</v>
       </c>
       <c r="J27" t="str">
-        <f>HEX2BIN(H27,3)</f>
+        <f t="shared" si="10"/>
         <v>000</v>
       </c>
       <c r="K27" t="str">
-        <f>HEX2BIN(I27,8)</f>
+        <f t="shared" si="11"/>
         <v>00001000</v>
       </c>
     </row>
-    <row r="28" spans="2:11">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
         <v>18</v>
       </c>
@@ -1316,107 +1316,107 @@
       </c>
       <c r="I28" s="2"/>
       <c r="J28" t="str">
-        <f>HEX2BIN(H28,3)</f>
+        <f t="shared" si="10"/>
         <v>010</v>
       </c>
       <c r="K28" t="str">
-        <f>HEX2BIN(I28,8)</f>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11">
+        <f t="shared" si="11"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.4">
       <c r="I29" s="2"/>
       <c r="J29" t="str">
-        <f>HEX2BIN(H29,3)</f>
+        <f t="shared" si="10"/>
         <v>000</v>
       </c>
       <c r="K29" t="str">
-        <f>HEX2BIN(I29,8)</f>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11">
+        <f t="shared" si="11"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.4">
       <c r="I30" s="2"/>
       <c r="J30" t="str">
-        <f>HEX2BIN(H30,3)</f>
+        <f t="shared" si="10"/>
         <v>000</v>
       </c>
       <c r="K30" t="str">
-        <f>HEX2BIN(I30,8)</f>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11">
+        <f t="shared" si="11"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J31" t="str">
-        <f t="shared" ref="J31:J46" si="10">HEX2BIN(H31,3)</f>
+        <f t="shared" ref="J31:J46" si="12">HEX2BIN(H31,3)</f>
         <v>000</v>
       </c>
       <c r="K31" t="str">
-        <f t="shared" ref="K31:K46" si="11">HEX2BIN(I31,8)</f>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11">
+        <f t="shared" ref="K31:K46" si="13">HEX2BIN(I31,8)</f>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J32" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K32" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J33" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K33" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J34" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K34" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J35" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J36" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J37" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K37" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B38" t="s">
         <v>23</v>
       </c>
@@ -1436,91 +1436,91 @@
         <v>2</v>
       </c>
       <c r="J38" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>111</v>
       </c>
       <c r="K38" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>00000010</v>
       </c>
     </row>
-    <row r="39" spans="2:11">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J39" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K39" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J40" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K40" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J41" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K41" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J42" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K42" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J43" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K43" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J44" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K44" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J45" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K45" t="str">
-        <f t="shared" si="11"/>
-        <v>00000000</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11">
+        <f t="shared" si="13"/>
+        <v>00000000</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.4">
       <c r="J46" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>000</v>
       </c>
       <c r="K46" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>00000000</v>
       </c>
     </row>
@@ -1535,6 +1535,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x0101005FC3FEB82594314CB0FECB3CD04E6E25" ma:contentTypeVersion="14" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="4392c6104558bcb855244c25c9dd78b9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="43cd1894-708a-4290-adf7-348d54d31837" xmlns:ns4="10495901-9a88-43e9-a0c2-59df6c25c8bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="810254e4ea0f8aee6c476eaa1feda21e" ns3:_="" ns4:_="">
     <xsd:import namespace="43cd1894-708a-4290-adf7-348d54d31837"/>
@@ -1763,36 +1778,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DDACDB-4B80-4995-81EB-8342A1C54290}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4BDA834-5B92-48FB-A6B0-E102C84F4220}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="43cd1894-708a-4290-adf7-348d54d31837"/>
-    <ds:schemaRef ds:uri="10495901-9a88-43e9-a0c2-59df6c25c8bf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1815,9 +1804,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4BDA834-5B92-48FB-A6B0-E102C84F4220}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DDACDB-4B80-4995-81EB-8342A1C54290}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="43cd1894-708a-4290-adf7-348d54d31837"/>
+    <ds:schemaRef ds:uri="10495901-9a88-43e9-a0c2-59df6c25c8bf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix a mistake that float is 8byte, actually4 byte
</commit_message>
<xml_diff>
--- a/R2CANIDList.xlsx
+++ b/R2CANIDList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tsemi\2023\ABURobocon2024\Software\NHK2024_R2CANIDList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05633631-D9C7-4B7A-AE73-112F6AC9B3CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA6E8F7-2D3C-462E-8DF0-8FA354F5BCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-6345" windowWidth="16440" windowHeight="29040" xr2:uid="{BB5A1F1B-FA35-4493-89FB-4447E27D9365}"/>
+    <workbookView xWindow="-16200" yWindow="-6225" windowWidth="16410" windowHeight="16305" xr2:uid="{BB5A1F1B-FA35-4493-89FB-4447E27D9365}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -732,7 +732,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -982,7 +982,7 @@
         <v>10</v>
       </c>
       <c r="F11">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="G11" t="s">
         <v>15</v>
@@ -1535,21 +1535,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x0101005FC3FEB82594314CB0FECB3CD04E6E25" ma:contentTypeVersion="14" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="4392c6104558bcb855244c25c9dd78b9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="43cd1894-708a-4290-adf7-348d54d31837" xmlns:ns4="10495901-9a88-43e9-a0c2-59df6c25c8bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="810254e4ea0f8aee6c476eaa1feda21e" ns3:_="" ns4:_="">
     <xsd:import namespace="43cd1894-708a-4290-adf7-348d54d31837"/>
@@ -1778,10 +1763,36 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4BDA834-5B92-48FB-A6B0-E102C84F4220}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DDACDB-4B80-4995-81EB-8342A1C54290}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="43cd1894-708a-4290-adf7-348d54d31837"/>
+    <ds:schemaRef ds:uri="10495901-9a88-43e9-a0c2-59df6c25c8bf"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1804,20 +1815,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3DDACDB-4B80-4995-81EB-8342A1C54290}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4BDA834-5B92-48FB-A6B0-E102C84F4220}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="43cd1894-708a-4290-adf7-348d54d31837"/>
-    <ds:schemaRef ds:uri="10495901-9a88-43e9-a0c2-59df6c25c8bf"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>